<commit_message>
Lots of little updates. Cleanup
</commit_message>
<xml_diff>
--- a/holdings/cnbs/03-08-21.xlsx
+++ b/holdings/cnbs/03-08-21.xlsx
@@ -506,7 +506,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -536,12 +536,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.640000</t>
+          <t>0.660000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>28257.27</t>
+          <t>29101.23</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -564,11 +564,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -598,22 +599,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>19.840000</t>
+          <t>20.460000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>9714766.73</t>
+          <t>10004917.40</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>7.91%</t>
+          <t>8.23%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -626,11 +627,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -660,22 +662,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>73.570000</t>
+          <t>71.460000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1139525.73</t>
+          <t>1106843.94</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.93%</t>
+          <t>0.91%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -688,11 +690,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,22 +725,22 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>18.090000</t>
+          <t>18.110000</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3738624.12</t>
+          <t>3742757.48</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3.04%</t>
+          <t>3.08%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -750,11 +753,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -784,12 +788,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>31.170000</t>
+          <t>30.860000</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>11764306.08</t>
+          <t>11647304.64</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -799,7 +803,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -812,11 +816,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -846,22 +851,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>12.160000</t>
+          <t>11.660000</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3598934.40</t>
+          <t>3450951.90</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2.93%</t>
+          <t>2.84%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -874,11 +879,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -908,22 +914,22 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>9.480000</t>
+          <t>9.440000</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5611960.92</t>
+          <t>5588281.76</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4.57%</t>
+          <t>4.60%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -936,11 +942,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -970,22 +977,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5.800000</t>
+          <t>5.510000</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3719541.51</t>
+          <t>3528825.51</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3.03%</t>
+          <t>2.90%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -998,11 +1005,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1032,22 +1040,22 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5.000000</t>
+          <t>5.010000</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2128625.00</t>
+          <t>2132882.25</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1.73%</t>
+          <t>1.75%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1060,11 +1068,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1094,22 +1103,22 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>40.400000</t>
+          <t>37.790000</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>3918113.20</t>
+          <t>3664987.57</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3.19%</t>
+          <t>3.01%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1122,11 +1131,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1156,22 +1166,22 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>214.940000</t>
+          <t>214.720000</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>14470620.56</t>
+          <t>14455809.28</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>11.78%</t>
+          <t>11.89%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1184,11 +1194,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1218,22 +1229,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>48.750000</t>
+          <t>47.420000</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>5735681.25</t>
+          <t>5579200.10</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4.67%</t>
+          <t>4.59%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1246,11 +1257,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1280,22 +1292,22 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>173.740000</t>
+          <t>165.650000</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>4346106.10</t>
+          <t>4143734.75</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>3.54%</t>
+          <t>3.41%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1308,11 +1320,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1322,7 +1335,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>IMCC</t>
+          <t>IMCC CN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1342,12 +1355,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>8.740000</t>
+          <t>10.200000</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>34520.89</t>
+          <t>40233.51</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1357,7 +1370,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1370,11 +1383,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1404,22 +1418,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>4.510000</t>
+          <t>4.780000</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>829010.16</t>
+          <t>878640.48</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>0.72%</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1432,11 +1446,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1466,22 +1481,22 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.485000</t>
+          <t>0.475000</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1302529.78</t>
+          <t>1273962.67</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1.06%</t>
+          <t>1.05%</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1494,11 +1509,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1528,12 +1544,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1.410000</t>
+          <t>1.390000</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1711683.60</t>
+          <t>1687404.40</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1543,7 +1559,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1556,11 +1572,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1590,22 +1607,22 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2.680000</t>
+          <t>2.830000</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2337394.16</t>
+          <t>2468218.46</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1.90%</t>
+          <t>2.03%</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1618,11 +1635,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1652,22 +1670,22 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>124.050000</t>
+          <t>121.560000</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>4426228.05</t>
+          <t>4337382.36</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>3.60%</t>
+          <t>3.57%</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1680,11 +1698,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1714,22 +1733,22 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2.840000</t>
+          <t>2.590000</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>7226805.02</t>
+          <t>6581803.79</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>5.88%</t>
+          <t>5.41%</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1742,11 +1761,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1776,22 +1796,22 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>18.250000</t>
+          <t>17.640000</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>9241800.00</t>
+          <t>8932896.00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>7.53%</t>
+          <t>7.35%</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1804,11 +1824,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1838,22 +1859,22 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>21.630000</t>
+          <t>22.420000</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1103649.12</t>
+          <t>1143958.08</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0.90%</t>
+          <t>0.94%</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1866,11 +1887,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1900,22 +1922,22 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>13.580000</t>
+          <t>13.750000</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>10353283.36</t>
+          <t>10482890.00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>8.43%</t>
+          <t>8.62%</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1928,11 +1950,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1942,7 +1965,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>VLNS</t>
+          <t>VLNS CN</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1962,12 +1985,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1.740000</t>
+          <t>1.700000</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>54980.65</t>
+          <t>53644.68</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1977,7 +2000,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1990,11 +2013,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2029,7 +2053,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>590159.85</t>
+          <t>589368.38</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2039,7 +2063,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2052,11 +2076,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2086,22 +2111,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>3.670000</t>
+          <t>3.960000</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1690310.25</t>
+          <t>1823877.00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>1.38%</t>
+          <t>1.50%</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2114,11 +2139,12 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/08/2021</t>
+          <t>03/09/2021</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2148,22 +2174,22 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>4.150000</t>
+          <t>4.140000</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1128733.60</t>
+          <t>1126013.76</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0.92%</t>
+          <t>0.93%</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>122813770.00</t>
+          <t>121588240.00</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2176,6 +2202,7 @@
           <t>89</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>